<commit_message>
Ultima versão com paretos atualizados no banco de dados Minitab Estratificações atualizadas Análise Financeira pronta para ser analisada
</commit_message>
<xml_diff>
--- a/Define/Custos Servidores/Relatório sobre custos.xlsx
+++ b/Define/Custos Servidores/Relatório sobre custos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Gerais" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>CUSTO MÉDIO TOTAL ANUAL</t>
   </si>
@@ -466,14 +466,18 @@
   <si>
     <t>PENDENTE DE ATUALIZAÇÃO DE VALORES</t>
   </si>
+  <si>
+    <t>*qual a produtividade do servidor /recursos(custos direto)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -805,7 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -881,49 +885,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -931,9 +893,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -969,6 +928,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2945,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2961,12 +2968,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3036,18 +3043,18 @@
       <c r="D6" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
+      <c r="A8" s="53"/>
       <c r="B8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3074,17 +3081,17 @@
       <c r="A11" s="33">
         <v>42</v>
       </c>
-      <c r="B11" s="63">
+      <c r="B11" s="48">
         <v>13408.36</v>
       </c>
-      <c r="C11" s="63">
+      <c r="C11" s="48">
         <v>160900.28</v>
       </c>
-      <c r="D11" s="64">
+      <c r="D11" s="49">
         <f>(B11/30)</f>
         <v>446.94533333333334</v>
       </c>
-      <c r="E11" s="65">
+      <c r="E11" s="50">
         <f>D11*3</f>
         <v>1340.836</v>
       </c>
@@ -3093,7 +3100,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="47" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3129,27 +3136,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="50"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="65"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3163,7 +3170,7 @@
       <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="55">
         <v>0.52439999999999998</v>
       </c>
       <c r="C4" s="38"/>
@@ -3175,16 +3182,16 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="42" t="s">
         <v>69</v>
       </c>
       <c r="G8" s="21" t="s">
@@ -3192,168 +3199,168 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="40">
         <v>44.73</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="40">
         <v>12.2</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="55">
+      <c r="G9" s="41">
         <f>SUM(C9:F9)</f>
         <v>56.929999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="40">
         <v>268.37</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="40">
         <v>17.079999999999998</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="40">
         <v>54.22</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="41">
         <f t="shared" ref="G10:G21" si="0">SUM(C10:F10)</f>
         <v>339.66999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="51" t="s">
+      <c r="A11" s="66"/>
+      <c r="B11" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="40">
         <v>268.37</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="40">
         <v>17.079999999999998</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="40">
         <v>54.22</v>
       </c>
-      <c r="G11" s="55">
+      <c r="G11" s="41">
         <f t="shared" si="0"/>
         <v>339.66999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="51" t="s">
+      <c r="A12" s="66"/>
+      <c r="B12" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="40">
         <v>223.64</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="40">
         <v>19.52</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="40">
         <v>54.22</v>
       </c>
-      <c r="G12" s="55">
+      <c r="G12" s="41">
         <f t="shared" si="0"/>
         <v>297.38</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="51" t="s">
+      <c r="A13" s="66"/>
+      <c r="B13" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="40">
         <v>313.10000000000002</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="40">
         <v>17.079999999999998</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="54">
+      <c r="F13" s="40">
         <v>54.22</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="41">
         <f t="shared" si="0"/>
         <v>384.4</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="51" t="s">
+      <c r="A14" s="66"/>
+      <c r="B14" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="40">
         <v>89.46</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="40">
         <v>1.22</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="40">
         <v>54.22</v>
       </c>
-      <c r="G14" s="55">
+      <c r="G14" s="41">
         <f t="shared" si="0"/>
         <v>144.89999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="52" t="s">
+      <c r="A15" s="66"/>
+      <c r="B15" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="40">
         <v>44.73</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="40">
         <v>19.52</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="55">
+      <c r="G15" s="41">
         <f t="shared" si="0"/>
         <v>64.25</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55">
+      <c r="A16" s="66"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3362,19 +3369,19 @@
       <c r="B17" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="40">
         <v>162.65</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="40">
         <v>1.22</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="40">
         <v>174.27</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="40">
         <v>7.75</v>
       </c>
-      <c r="G17" s="55">
+      <c r="G17" s="41">
         <f t="shared" si="0"/>
         <v>345.89</v>
       </c>
@@ -3383,20 +3390,20 @@
       <c r="B18" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="40">
         <v>284.64</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="40">
         <v>284.41000000000003</v>
       </c>
-      <c r="E18" s="69">
+      <c r="E18" s="54">
         <f>SUM(2439.75,1742.68)</f>
         <v>4182.43</v>
       </c>
-      <c r="F18" s="54">
+      <c r="F18" s="40">
         <v>3.87</v>
       </c>
-      <c r="G18" s="55">
+      <c r="G18" s="41">
         <f t="shared" si="0"/>
         <v>4755.3500000000004</v>
       </c>
@@ -3405,19 +3412,19 @@
       <c r="B19" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="40">
         <v>81.319999999999993</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="40">
         <v>43.92</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="40">
         <v>43.57</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="40">
         <v>3.87</v>
       </c>
-      <c r="G19" s="55">
+      <c r="G19" s="41">
         <f t="shared" si="0"/>
         <v>172.68</v>
       </c>
@@ -3426,19 +3433,19 @@
       <c r="B20" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="40">
         <v>121.99</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="40">
         <v>29.28</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="40">
         <v>174.27</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="40">
         <v>15.49</v>
       </c>
-      <c r="G20" s="55">
+      <c r="G20" s="41">
         <f t="shared" si="0"/>
         <v>341.03</v>
       </c>
@@ -3447,44 +3454,44 @@
       <c r="B21" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="40">
         <v>203.31</v>
       </c>
-      <c r="D21" s="54">
+      <c r="D21" s="40">
         <v>26.84</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="40">
         <v>58.09</v>
       </c>
-      <c r="F21" s="54">
+      <c r="F21" s="40">
         <v>7.75</v>
       </c>
-      <c r="G21" s="55">
+      <c r="G21" s="41">
         <f t="shared" si="0"/>
         <v>295.99</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="58">
+      <c r="C22" s="44">
         <f>SUM(C9:C21)</f>
         <v>2106.31</v>
       </c>
-      <c r="D22" s="58">
+      <c r="D22" s="44">
         <f t="shared" ref="D22:F22" si="1">SUM(D9:D21)</f>
         <v>489.37000000000006</v>
       </c>
-      <c r="E22" s="58">
+      <c r="E22" s="44">
         <f t="shared" si="1"/>
         <v>4632.630000000001</v>
       </c>
-      <c r="F22" s="58">
+      <c r="F22" s="44">
         <f t="shared" si="1"/>
         <v>309.83000000000004</v>
       </c>
-      <c r="G22" s="58">
+      <c r="G22" s="44">
         <f>SUM(G9:G21)</f>
         <v>7538.14</v>
       </c>
@@ -3508,8 +3515,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,22 +3541,22 @@
       <c r="C2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="44"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -3560,10 +3567,10 @@
         <v>35</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="47">
+      <c r="H5" s="76">
         <v>0.15</v>
       </c>
-      <c r="I5" s="46"/>
+      <c r="I5" s="75"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -3581,10 +3588,10 @@
       <c r="F6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="44"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3602,10 +3609,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="46"/>
+      <c r="I7" s="75"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -3623,10 +3630,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="44"/>
+      <c r="I8" s="72"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -3644,18 +3651,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="46"/>
+      <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -3664,36 +3671,36 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -3727,7 +3734,7 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="74" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3745,7 +3752,7 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
@@ -3761,8 +3768,8 @@
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="59" t="s">
+      <c r="A18" s="74"/>
+      <c r="B18" s="45" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="18"/>
@@ -3831,9 +3838,12 @@
         <f>C20/12</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="E20" s="14">
-        <f>D20/30</f>
-        <v>0.1388888888888889</v>
+      <c r="E20" s="77">
+        <f>(D20/30)/100</f>
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="8"/>
@@ -3852,19 +3862,19 @@
       </c>
       <c r="E21" s="14">
         <f>E20*E19</f>
-        <v>74.095205555555552</v>
+        <v>0.74095205555555554</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
@@ -3897,8 +3907,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3923,26 +3933,26 @@
       <c r="C2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="44"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
+      <c r="A3" s="53"/>
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -3953,10 +3963,10 @@
         <v>35</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="47">
+      <c r="H5" s="76">
         <v>0.15</v>
       </c>
-      <c r="I5" s="46"/>
+      <c r="I5" s="75"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -3974,10 +3984,10 @@
       <c r="F6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="44"/>
+      <c r="I6" s="72"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3995,10 +4005,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="46"/>
+      <c r="I7" s="75"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4016,10 +4026,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="44"/>
+      <c r="I8" s="72"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4037,18 +4047,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="46"/>
+      <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -4057,36 +4067,36 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -4106,60 +4116,60 @@
       <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="71">
+      <c r="C15" s="56">
         <f>'Dados Gerais'!C11</f>
         <v>160900.28</v>
       </c>
-      <c r="D15" s="72">
+      <c r="D15" s="57">
         <f>'Dados Gerais'!B3</f>
         <v>13408.36</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="58">
         <f>D15/30</f>
         <v>446.94533333333334</v>
       </c>
-      <c r="F15" s="62" t="s">
+      <c r="F15" s="47" t="s">
         <v>74</v>
       </c>
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="74" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="75">
+      <c r="C16" s="59"/>
+      <c r="D16" s="60">
         <f>CustosDiretos!C22</f>
         <v>2106.31</v>
       </c>
-      <c r="E16" s="74">
+      <c r="E16" s="59">
         <f>D16/30</f>
         <v>70.210333333333338</v>
       </c>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75">
+      <c r="C17" s="59"/>
+      <c r="D17" s="60">
         <f>CustosDiretos!D22</f>
         <v>489.37000000000006</v>
       </c>
-      <c r="E17" s="74">
+      <c r="E17" s="59">
         <f>D17/30</f>
         <v>16.312333333333335</v>
       </c>
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="59" t="s">
+      <c r="A18" s="74"/>
+      <c r="B18" s="45" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="18"/>
@@ -4200,19 +4210,19 @@
         <f>SUM(E15:E18)</f>
         <v>533.48547999999994</v>
       </c>
-      <c r="F19" s="66">
+      <c r="F19" s="51">
         <f>E19*3</f>
         <v>1600.4564399999999</v>
       </c>
-      <c r="G19" s="67">
+      <c r="G19" s="52">
         <f>C20*3</f>
         <v>150</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="51">
         <f>E19*G19</f>
         <v>80022.821999999986</v>
       </c>
-      <c r="I19" s="66">
+      <c r="I19" s="51">
         <f>42*H19</f>
         <v>3360958.5239999993</v>
       </c>
@@ -4239,40 +4249,35 @@
       <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="76">
+      <c r="C21" s="61">
         <f>C20*C19</f>
         <v>8045014</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="61">
         <f>D20*D19</f>
         <v>66685.685000000012</v>
       </c>
-      <c r="E21" s="76">
+      <c r="E21" s="61">
         <f>E20*E19</f>
         <v>74.095205555555552</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:I13"/>
-    <mergeCell ref="A16:A18"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
@@ -4280,6 +4285,11 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:I13"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ultimas atualizações Apresentação Analyze
</commit_message>
<xml_diff>
--- a/Define/Custos Servidores/Relatório sobre custos.xlsx
+++ b/Define/Custos Servidores/Relatório sobre custos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Gerais" sheetId="1" r:id="rId1"/>
@@ -203,12 +203,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>CUSTO MÉDIO TOTAL ANUAL</t>
-  </si>
-  <si>
-    <t>CUSTO SALARIAL - SERVIDORES DA SECGS</t>
   </si>
   <si>
     <t>TELEFONE</t>
@@ -279,9 +276,6 @@
   </si>
   <si>
     <t>MÉDIA  DE DIAS EM TRÂMITE DA SECGS ATUAL</t>
-  </si>
-  <si>
-    <t>18 DIAS</t>
   </si>
   <si>
     <t>META DE REDUÇÃO GERAL</t>
@@ -458,28 +452,48 @@
     <t>CUSTO SALARIAL LÍQUIDO- SERVIDORES DA SECGS</t>
   </si>
   <si>
-    <t>*Atualizar para valores calculados considerando os impostos que incidem sobre o salário</t>
-  </si>
-  <si>
     <t>PENDENTE DE ATUALIZAÇÃO DOS DADOS CALCULADOS COM OS IMPOSTOS</t>
   </si>
   <si>
-    <t>PENDENTE DE ATUALIZAÇÃO DE VALORES</t>
-  </si>
-  <si>
     <t>*qual a produtividade do servidor /recursos(custos direto)</t>
+  </si>
+  <si>
+    <t>CUSTO SALARIAL BRUTO- SERVIDORES DA SECGS</t>
+  </si>
+  <si>
+    <t>Descontado 23,6% do valor mensal</t>
+  </si>
+  <si>
+    <t>CUSTO MÉDIO MENSAL LÍQUIDO
+1 SERVIDOR</t>
+  </si>
+  <si>
+    <t>ATUALIZADO COM -23,6%</t>
+  </si>
+  <si>
+    <t>ATUALIZADO COM DESCONTO DE 23,6%</t>
+  </si>
+  <si>
+    <t>21 DIAS</t>
+  </si>
+  <si>
+    <t>DIFERENÇA(LÍQUIDO - BRUTO)</t>
+  </si>
+  <si>
+    <t>18 DIAS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,8 +597,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +652,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -909,7 +943,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -930,6 +963,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -975,8 +1012,17 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2952,8 +2998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,32 +3010,32 @@
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="A1" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -3014,7 +3060,7 @@
         <f>D3*3</f>
         <v>1340.836</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="78">
         <v>6757811.6699999999</v>
       </c>
     </row>
@@ -3022,7 +3068,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -3034,7 +3080,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1">
         <v>431</v>
@@ -3043,34 +3089,44 @@
       <c r="D6" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="62"/>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="F8" s="79" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="80">
+        <f>F11-F3</f>
+        <v>-1164594.7461599996</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
+      <c r="A9" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>0</v>
@@ -3082,27 +3138,28 @@
         <v>42</v>
       </c>
       <c r="B11" s="48">
-        <v>13408.36</v>
+        <f>B3-(13408.36 *23.6%)</f>
+        <v>10243.98704</v>
       </c>
       <c r="C11" s="48">
-        <v>160900.28</v>
+        <f>B11*13</f>
+        <v>133171.83152000001</v>
       </c>
       <c r="D11" s="49">
         <f>(B11/30)</f>
-        <v>446.94533333333334</v>
+        <v>341.46623466666665</v>
       </c>
       <c r="E11" s="50">
         <f>D11*3</f>
-        <v>1340.836</v>
-      </c>
-      <c r="F11" s="5">
-        <v>6757811.6699999999</v>
+        <v>1024.398704</v>
+      </c>
+      <c r="F11" s="78">
+        <f>C11*42</f>
+        <v>5593216.9238400003</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="47" t="s">
-        <v>77</v>
-      </c>
+      <c r="C13" s="81"/>
     </row>
     <row r="14" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3121,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,41 +3193,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="65"/>
+      <c r="A1" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="66"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="55">
+        <v>38</v>
+      </c>
+      <c r="B4" s="54">
         <v>0.52439999999999998</v>
       </c>
       <c r="C4" s="38"/>
@@ -3178,29 +3235,29 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="42" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F8" s="42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="40">
         <v>44.73</v>
@@ -3209,10 +3266,10 @@
         <v>12.2</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" s="41">
         <f>SUM(C9:F9)</f>
@@ -3220,11 +3277,11 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
-        <v>53</v>
+      <c r="A10" s="67" t="s">
+        <v>51</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" s="40">
         <v>268.37</v>
@@ -3233,7 +3290,7 @@
         <v>17.079999999999998</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F10" s="40">
         <v>54.22</v>
@@ -3244,9 +3301,9 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="40">
         <v>268.37</v>
@@ -3255,7 +3312,7 @@
         <v>17.079999999999998</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" s="40">
         <v>54.22</v>
@@ -3266,9 +3323,9 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="40">
         <v>223.64</v>
@@ -3277,7 +3334,7 @@
         <v>19.52</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F12" s="40">
         <v>54.22</v>
@@ -3288,9 +3345,9 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="40">
         <v>313.10000000000002</v>
@@ -3299,7 +3356,7 @@
         <v>17.079999999999998</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F13" s="40">
         <v>54.22</v>
@@ -3310,9 +3367,9 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="40">
         <v>89.46</v>
@@ -3321,7 +3378,7 @@
         <v>1.22</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F14" s="40">
         <v>54.22</v>
@@ -3332,9 +3389,9 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="67" t="s">
-        <v>53</v>
+      <c r="A15" s="67"/>
+      <c r="B15" s="68" t="s">
+        <v>51</v>
       </c>
       <c r="C15" s="40">
         <v>44.73</v>
@@ -3343,10 +3400,10 @@
         <v>19.52</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" s="41">
         <f t="shared" si="0"/>
@@ -3354,8 +3411,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="67"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -3367,7 +3424,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" s="40">
         <v>162.65</v>
@@ -3388,7 +3445,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" s="40">
         <v>284.64</v>
@@ -3396,7 +3453,7 @@
       <c r="D18" s="40">
         <v>284.41000000000003</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="53">
         <f>SUM(2439.75,1742.68)</f>
         <v>4182.43</v>
       </c>
@@ -3410,7 +3467,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="40">
         <v>81.319999999999993</v>
@@ -3431,7 +3488,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="40">
         <v>121.99</v>
@@ -3452,7 +3509,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="40">
         <v>203.31</v>
@@ -3473,7 +3530,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="44">
         <f>SUM(C9:C21)</f>
@@ -3515,8 +3572,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3534,64 +3591,64 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="73"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="76"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="75"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="72"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="76">
+      <c r="H5" s="77">
         <v>0.15</v>
       </c>
-      <c r="I5" s="75"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="72"/>
+      <c r="H6" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="73"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3609,10 +3666,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="75"/>
+      <c r="H7" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="76"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -3630,10 +3687,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="72"/>
+      <c r="H8" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="73"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -3651,18 +3708,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="75" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="75"/>
+      <c r="H9" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
+      <c r="B10" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -3671,54 +3728,54 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
+      <c r="B11" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="24" t="s">
         <v>14</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>15</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="18">
         <v>160900.28</v>
@@ -3734,11 +3791,11 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
-        <v>12</v>
+      <c r="A16" s="75" t="s">
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19">
@@ -3752,9 +3809,9 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19">
@@ -3768,9 +3825,9 @@
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19">
@@ -3782,21 +3839,21 @@
         <v>1.7479999999999999E-2</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="34" t="s">
         <v>16</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="16">
         <f>SUM(C15:C18)</f>
@@ -3829,7 +3886,7 @@
     </row>
     <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="14">
         <v>50</v>
@@ -3838,19 +3895,19 @@
         <f>C20/12</f>
         <v>4.166666666666667</v>
       </c>
-      <c r="E20" s="77">
+      <c r="E20" s="61">
         <f>(D20/30)/100</f>
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="14">
         <f>C20*C19</f>
@@ -3867,14 +3924,14 @@
     </row>
     <row r="22" spans="1:9" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
+        <v>50</v>
+      </c>
+      <c r="B22" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
@@ -3907,8 +3964,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,68 +3983,68 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="73"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="62"/>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="76"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="72"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="75" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="75"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="72" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="72"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="76">
+      <c r="H5" s="77">
         <v>0.15</v>
       </c>
-      <c r="I5" s="75"/>
+      <c r="I5" s="76"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="72"/>
+      <c r="H6" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="73"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -4005,10 +4062,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="75"/>
+      <c r="H7" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="76"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4026,10 +4083,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="72"/>
+      <c r="H8" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="73"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4047,18 +4104,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="75" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="75"/>
+      <c r="H9" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
+      <c r="B10" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -4067,110 +4124,110 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
+      <c r="B11" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="24" t="s">
         <v>14</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>15</v>
       </c>
       <c r="H14" s="26"/>
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="55">
+        <f>'Dados Gerais'!C11</f>
+        <v>133171.83152000001</v>
+      </c>
+      <c r="D15" s="56">
+        <f>'Dados Gerais'!B11</f>
+        <v>10243.98704</v>
+      </c>
+      <c r="E15" s="57">
+        <f>D15/30</f>
+        <v>341.46623466666665</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="56">
-        <f>'Dados Gerais'!C11</f>
-        <v>160900.28</v>
-      </c>
-      <c r="D15" s="57">
-        <f>'Dados Gerais'!B3</f>
-        <v>13408.36</v>
-      </c>
-      <c r="E15" s="58">
-        <f>D15/30</f>
-        <v>446.94533333333334</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" s="28"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60">
+      <c r="C16" s="58"/>
+      <c r="D16" s="59">
         <f>CustosDiretos!C22</f>
         <v>2106.31</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="58">
         <f>D16/30</f>
         <v>70.210333333333338</v>
       </c>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="74"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60">
+        <v>9</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59">
         <f>CustosDiretos!D22</f>
         <v>489.37000000000006</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="58">
         <f>D17/30</f>
         <v>16.312333333333335</v>
       </c>
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="74"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19">
@@ -4182,37 +4239,37 @@
         <v>1.7479999999999999E-2</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="34" t="s">
         <v>16</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="16">
         <f>SUM(C15:C18)</f>
-        <v>160900.28</v>
+        <v>133171.83152000001</v>
       </c>
       <c r="D19" s="17">
         <f>SUM(D15:D18)</f>
-        <v>16004.564400000001</v>
+        <v>12840.191440000001</v>
       </c>
       <c r="E19" s="16">
         <f>SUM(E15:E18)</f>
-        <v>533.48547999999994</v>
+        <v>428.00638133333331</v>
       </c>
       <c r="F19" s="51">
         <f>E19*3</f>
-        <v>1600.4564399999999</v>
+        <v>1284.0191439999999</v>
       </c>
       <c r="G19" s="52">
         <f>C20*3</f>
@@ -4220,16 +4277,16 @@
       </c>
       <c r="H19" s="51">
         <f>E19*G19</f>
-        <v>80022.821999999986</v>
+        <v>64200.957199999997</v>
       </c>
       <c r="I19" s="51">
         <f>42*H19</f>
-        <v>3360958.5239999993</v>
+        <v>2696440.2023999998</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="14">
         <v>50</v>
@@ -4247,37 +4304,38 @@
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="61">
+        <v>18</v>
+      </c>
+      <c r="C21" s="60">
         <f>C20*C19</f>
-        <v>8045014</v>
-      </c>
-      <c r="D21" s="61">
+        <v>6658591.5760000004</v>
+      </c>
+      <c r="D21" s="60">
         <f>D20*D19</f>
-        <v>66685.685000000012</v>
-      </c>
-      <c r="E21" s="61">
+        <v>53500.797666666673</v>
+      </c>
+      <c r="E21" s="60">
         <f>E20*E19</f>
-        <v>74.095205555555552</v>
+        <v>59.445330740740737</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
+        <v>50</v>
+      </c>
+      <c r="B22" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
@@ -4289,7 +4347,6 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:I13"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4317,73 +4374,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>40</v>
-      </c>
       <c r="C1" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="30">
         <v>42</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="31">
         <v>14500</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="31">
         <v>174000</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="31">
         <v>22.02</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="30"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="31">
         <v>0.83</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="30"/>
     </row>

</xml_diff>

<commit_message>
Atualização de vários docs e apresentação do Analyze
</commit_message>
<xml_diff>
--- a/Define/Custos Servidores/Relatório sobre custos.xlsx
+++ b/Define/Custos Servidores/Relatório sobre custos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11190" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dados Gerais" sheetId="1" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>CUSTO MÉDIO TOTAL ANUAL</t>
   </si>
@@ -482,6 +482,9 @@
   <si>
     <t>18 DIAS</t>
   </si>
+  <si>
+    <t>3 dias * (Média anual PAD)*(CUSTO DIARIO SERVIDOR)</t>
+  </si>
 </sst>
 </file>
 
@@ -491,7 +494,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="&quot;R$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -967,6 +970,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1011,18 +1026,6 @@
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3014,12 +3017,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3060,7 +3063,7 @@
         <f>D3*3</f>
         <v>1340.836</v>
       </c>
-      <c r="F3" s="78">
+      <c r="F3" s="63">
         <v>6757811.6699999999</v>
       </c>
     </row>
@@ -3093,21 +3096,21 @@
       <c r="B8" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="80">
+      <c r="G8" s="65">
         <f>F11-F3</f>
         <v>-1164594.7461599996</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
       <c r="E9" t="s">
         <v>78</v>
       </c>
@@ -3153,13 +3156,13 @@
         <f>D11*3</f>
         <v>1024.398704</v>
       </c>
-      <c r="F11" s="78">
+      <c r="F11" s="63">
         <f>C11*42</f>
         <v>5593216.9238400003</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="81"/>
+      <c r="C13" s="66"/>
     </row>
     <row r="14" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3193,27 +3196,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="66"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="70"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -3277,7 +3280,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="71" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="39" t="s">
@@ -3301,7 +3304,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="39" t="s">
         <v>55</v>
       </c>
@@ -3323,7 +3326,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
+      <c r="A12" s="71"/>
       <c r="B12" s="39" t="s">
         <v>56</v>
       </c>
@@ -3345,7 +3348,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
+      <c r="A13" s="71"/>
       <c r="B13" s="39" t="s">
         <v>57</v>
       </c>
@@ -3367,7 +3370,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="39" t="s">
         <v>58</v>
       </c>
@@ -3389,8 +3392,8 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
-      <c r="B15" s="68" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="72" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="40">
@@ -3411,8 +3414,8 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
-      <c r="B16" s="68"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="40"/>
       <c r="D16" s="40"/>
       <c r="E16" s="40"/>
@@ -3598,22 +3601,22 @@
       <c r="C2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="73"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="76"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="73"/>
+      <c r="I4" s="77"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -3624,10 +3627,10 @@
         <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="77">
+      <c r="H5" s="81">
         <v>0.15</v>
       </c>
-      <c r="I5" s="76"/>
+      <c r="I5" s="80"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -3645,10 +3648,10 @@
       <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="73"/>
+      <c r="I6" s="77"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -3666,10 +3669,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="76"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -3687,10 +3690,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="73"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -3708,18 +3711,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="76"/>
+      <c r="I9" s="80"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="72"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -3728,36 +3731,36 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -3791,7 +3794,7 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="79" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3809,7 +3812,7 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
+      <c r="A17" s="79"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -3825,7 +3828,7 @@
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="45" t="s">
         <v>1</v>
       </c>
@@ -3926,12 +3929,12 @@
       <c r="A22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
@@ -3964,8 +3967,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3990,26 +3993,26 @@
       <c r="C2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="73"/>
+      <c r="I2" s="77"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="62"/>
       <c r="B3" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="H3" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="76"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="73"/>
+      <c r="I4" s="77"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -4020,10 +4023,10 @@
         <v>33</v>
       </c>
       <c r="E5"/>
-      <c r="H5" s="77">
+      <c r="H5" s="81">
         <v>0.15</v>
       </c>
-      <c r="I5" s="76"/>
+      <c r="I5" s="80"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
@@ -4041,10 +4044,10 @@
       <c r="F6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="73"/>
+      <c r="I6" s="77"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -4062,10 +4065,10 @@
       <c r="F7" s="1">
         <v>33</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="76"/>
+      <c r="I7" s="80"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -4083,10 +4086,10 @@
       <c r="F8" s="1">
         <v>51</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="73"/>
+      <c r="I8" s="77"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -4104,18 +4107,18 @@
       <c r="F9" s="1">
         <v>67</v>
       </c>
-      <c r="H9" s="76" t="s">
+      <c r="H9" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="76"/>
+      <c r="I9" s="80"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="72"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="25">
         <f>ROUND(AVERAGE(33,51,67),0)</f>
         <v>50</v>
@@ -4124,36 +4127,36 @@
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
     </row>
     <row r="14" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
@@ -4191,7 +4194,7 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="79" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -4209,7 +4212,7 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="75"/>
+      <c r="A17" s="79"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -4225,7 +4228,7 @@
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="75"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="45" t="s">
         <v>1</v>
       </c>
@@ -4299,8 +4302,14 @@
         <f>D20/30</f>
         <v>0.1388888888888889</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="H20" s="8"/>
+      <c r="I20" s="8">
+        <f>(3*(1320))*E19</f>
+        <v>1694905.2700799999</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
@@ -4323,12 +4332,12 @@
       <c r="A22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>

</xml_diff>